<commit_message>
Data updated till 1/24/2022
</commit_message>
<xml_diff>
--- a/data/HAB_resolvablelakes_2022.xlsx
+++ b/data/HAB_resolvablelakes_2022.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L232"/>
+  <dimension ref="A1:L340"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8818,7 +8818,6 @@
       <c r="C226" t="n">
         <v>4680000</v>
       </c>
-      <c r="D226" t="inlineStr"/>
       <c r="E226" t="n">
         <v>6309.57666016</v>
       </c>
@@ -8856,7 +8855,6 @@
       <c r="C227" t="n">
         <v>1440000</v>
       </c>
-      <c r="D227" t="inlineStr"/>
       <c r="E227" t="n">
         <v>6309.57666016</v>
       </c>
@@ -8894,7 +8892,6 @@
       <c r="C228" t="n">
         <v>5760000</v>
       </c>
-      <c r="D228" t="inlineStr"/>
       <c r="E228" t="n">
         <v>6309.57666016</v>
       </c>
@@ -8932,7 +8929,6 @@
       <c r="C229" t="n">
         <v>26550000</v>
       </c>
-      <c r="D229" t="inlineStr"/>
       <c r="E229" t="n">
         <v>6309.57666016</v>
       </c>
@@ -8970,7 +8966,6 @@
       <c r="C230" t="n">
         <v>49410000</v>
       </c>
-      <c r="D230" t="inlineStr"/>
       <c r="E230" t="n">
         <v>6309.57666016</v>
       </c>
@@ -9008,7 +9003,6 @@
       <c r="C231" t="n">
         <v>4320000</v>
       </c>
-      <c r="D231" t="inlineStr"/>
       <c r="E231" t="n">
         <v>6309.57666016</v>
       </c>
@@ -9046,7 +9040,6 @@
       <c r="C232" t="n">
         <v>10890000</v>
       </c>
-      <c r="D232" t="inlineStr"/>
       <c r="E232" t="n">
         <v>6309.57666016</v>
       </c>
@@ -9070,6 +9063,4029 @@
       </c>
       <c r="L232" s="12" t="n">
         <v>44580</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Alkali Lake_01116863</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>27</v>
+      </c>
+      <c r="C233" t="n">
+        <v>2430000</v>
+      </c>
+      <c r="E233" t="n">
+        <v>151356.234375</v>
+      </c>
+      <c r="F233" t="n">
+        <v>1819701.875</v>
+      </c>
+      <c r="G233" t="n">
+        <v>1668345.64062</v>
+      </c>
+      <c r="H233" t="n">
+        <v>677569.519097</v>
+      </c>
+      <c r="I233" t="n">
+        <v>434939.809088</v>
+      </c>
+      <c r="J233" t="n">
+        <v>20</v>
+      </c>
+      <c r="K233" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L233" s="12" t="n">
+        <v>44581</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Renner Lake_00267175</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>3</v>
+      </c>
+      <c r="C234" t="n">
+        <v>270000</v>
+      </c>
+      <c r="E234" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F234" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G234" t="n">
+        <v>0</v>
+      </c>
+      <c r="H234" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I234" t="n">
+        <v>0</v>
+      </c>
+      <c r="J234" t="n">
+        <v>20</v>
+      </c>
+      <c r="K234" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L234" s="12" t="n">
+        <v>44581</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Summer Lake_01150595</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>82</v>
+      </c>
+      <c r="C235" t="n">
+        <v>7380000</v>
+      </c>
+      <c r="E235" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F235" t="n">
+        <v>164437.203125</v>
+      </c>
+      <c r="G235" t="n">
+        <v>158127.626465</v>
+      </c>
+      <c r="H235" t="n">
+        <v>34218.3198599</v>
+      </c>
+      <c r="I235" t="n">
+        <v>41925.8279688</v>
+      </c>
+      <c r="J235" t="n">
+        <v>20</v>
+      </c>
+      <c r="K235" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L235" s="12" t="n">
+        <v>44581</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Warm Springs Reservoir_01128656</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>76</v>
+      </c>
+      <c r="C236" t="n">
+        <v>6840000</v>
+      </c>
+      <c r="E236" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F236" t="n">
+        <v>164437.203125</v>
+      </c>
+      <c r="G236" t="n">
+        <v>158127.626465</v>
+      </c>
+      <c r="H236" t="n">
+        <v>11284.3450799</v>
+      </c>
+      <c r="I236" t="n">
+        <v>21810.9938338</v>
+      </c>
+      <c r="J236" t="n">
+        <v>21</v>
+      </c>
+      <c r="K236" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L236" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Beulah Reservoir_01117569</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>39</v>
+      </c>
+      <c r="C237" t="n">
+        <v>3510000</v>
+      </c>
+      <c r="E237" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F237" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G237" t="n">
+        <v>0</v>
+      </c>
+      <c r="H237" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I237" t="n">
+        <v>0</v>
+      </c>
+      <c r="J237" t="n">
+        <v>21</v>
+      </c>
+      <c r="K237" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L237" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Waldo Lake_01151818</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>102</v>
+      </c>
+      <c r="C238" t="n">
+        <v>9180000</v>
+      </c>
+      <c r="E238" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F238" t="n">
+        <v>376704</v>
+      </c>
+      <c r="G238" t="n">
+        <v>370394.42334</v>
+      </c>
+      <c r="H238" t="n">
+        <v>23228.9008693</v>
+      </c>
+      <c r="I238" t="n">
+        <v>49668.2749133</v>
+      </c>
+      <c r="J238" t="n">
+        <v>21</v>
+      </c>
+      <c r="K238" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L238" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Cold Springs Reservoir_01119125</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>27</v>
+      </c>
+      <c r="C239" t="n">
+        <v>2430000</v>
+      </c>
+      <c r="E239" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F239" t="n">
+        <v>92045</v>
+      </c>
+      <c r="G239" t="n">
+        <v>85735.42333980001</v>
+      </c>
+      <c r="H239" t="n">
+        <v>12560.8479456</v>
+      </c>
+      <c r="I239" t="n">
+        <v>20268.0882791</v>
+      </c>
+      <c r="J239" t="n">
+        <v>21</v>
+      </c>
+      <c r="K239" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L239" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Crescent Lake_01158186</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>58</v>
+      </c>
+      <c r="C240" t="n">
+        <v>5220000</v>
+      </c>
+      <c r="E240" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F240" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G240" t="n">
+        <v>0</v>
+      </c>
+      <c r="H240" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I240" t="n">
+        <v>0</v>
+      </c>
+      <c r="J240" t="n">
+        <v>21</v>
+      </c>
+      <c r="K240" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L240" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Wickiup Reservoir_01161711</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>13</v>
+      </c>
+      <c r="C241" t="n">
+        <v>1170000</v>
+      </c>
+      <c r="E241" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F241" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G241" t="n">
+        <v>0</v>
+      </c>
+      <c r="H241" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I241" t="n">
+        <v>0</v>
+      </c>
+      <c r="J241" t="n">
+        <v>21</v>
+      </c>
+      <c r="K241" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L241" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Paulina Lake_01147502</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>43</v>
+      </c>
+      <c r="C242" t="n">
+        <v>3870000</v>
+      </c>
+      <c r="E242" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F242" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G242" t="n">
+        <v>0</v>
+      </c>
+      <c r="H242" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I242" t="n">
+        <v>0</v>
+      </c>
+      <c r="J242" t="n">
+        <v>21</v>
+      </c>
+      <c r="K242" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L242" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Odell Lake_01147159</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>13</v>
+      </c>
+      <c r="C243" t="n">
+        <v>1170000</v>
+      </c>
+      <c r="E243" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F243" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G243" t="n">
+        <v>0</v>
+      </c>
+      <c r="H243" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I243" t="n">
+        <v>0</v>
+      </c>
+      <c r="J243" t="n">
+        <v>21</v>
+      </c>
+      <c r="K243" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L243" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Hills Creek Lake_01158881</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>21</v>
+      </c>
+      <c r="C244" t="n">
+        <v>1890000</v>
+      </c>
+      <c r="E244" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F244" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G244" t="n">
+        <v>0</v>
+      </c>
+      <c r="H244" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I244" t="n">
+        <v>0</v>
+      </c>
+      <c r="J244" t="n">
+        <v>21</v>
+      </c>
+      <c r="K244" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L244" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Lost Creek Lake_01158890</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>83</v>
+      </c>
+      <c r="C245" t="n">
+        <v>7470000</v>
+      </c>
+      <c r="E245" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F245" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G245" t="n">
+        <v>0</v>
+      </c>
+      <c r="H245" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I245" t="n">
+        <v>0</v>
+      </c>
+      <c r="J245" t="n">
+        <v>21</v>
+      </c>
+      <c r="K245" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L245" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Malheur Lake_01123710</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>571</v>
+      </c>
+      <c r="C246" t="n">
+        <v>51390000</v>
+      </c>
+      <c r="E246" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F246" t="n">
+        <v>216770.515625</v>
+      </c>
+      <c r="G246" t="n">
+        <v>210460.938965</v>
+      </c>
+      <c r="H246" t="n">
+        <v>40766.3185347</v>
+      </c>
+      <c r="I246" t="n">
+        <v>44794.5575758</v>
+      </c>
+      <c r="J246" t="n">
+        <v>21</v>
+      </c>
+      <c r="K246" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L246" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Foster Lake_01158892</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>22</v>
+      </c>
+      <c r="C247" t="n">
+        <v>1980000</v>
+      </c>
+      <c r="E247" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F247" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G247" t="n">
+        <v>0</v>
+      </c>
+      <c r="H247" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I247" t="n">
+        <v>0</v>
+      </c>
+      <c r="J247" t="n">
+        <v>21</v>
+      </c>
+      <c r="K247" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L247" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Goose Lake_00224325</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>441</v>
+      </c>
+      <c r="C248" t="n">
+        <v>39690000</v>
+      </c>
+      <c r="E248" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F248" t="n">
+        <v>235505.046875</v>
+      </c>
+      <c r="G248" t="n">
+        <v>229195.470215</v>
+      </c>
+      <c r="H248" t="n">
+        <v>19374.2736412</v>
+      </c>
+      <c r="I248" t="n">
+        <v>33268.5641673</v>
+      </c>
+      <c r="J248" t="n">
+        <v>21</v>
+      </c>
+      <c r="K248" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L248" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Crump Lake_01119601</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>6</v>
+      </c>
+      <c r="C249" t="n">
+        <v>540000</v>
+      </c>
+      <c r="E249" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F249" t="n">
+        <v>75857.78125</v>
+      </c>
+      <c r="G249" t="n">
+        <v>69548.20458980001</v>
+      </c>
+      <c r="H249" t="n">
+        <v>34160.8898112</v>
+      </c>
+      <c r="I249" t="n">
+        <v>28734.3522125</v>
+      </c>
+      <c r="J249" t="n">
+        <v>21</v>
+      </c>
+      <c r="K249" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L249" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Upper Klamath Lake_01151685</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C250" t="n">
+        <v>181620000</v>
+      </c>
+      <c r="E250" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F250" t="n">
+        <v>398107.53125</v>
+      </c>
+      <c r="G250" t="n">
+        <v>391797.95459</v>
+      </c>
+      <c r="H250" t="n">
+        <v>14340.0780984</v>
+      </c>
+      <c r="I250" t="n">
+        <v>30221.8318849</v>
+      </c>
+      <c r="J250" t="n">
+        <v>21</v>
+      </c>
+      <c r="K250" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L250" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Henry Hagg Lake_01158095</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>27</v>
+      </c>
+      <c r="C251" t="n">
+        <v>2430000</v>
+      </c>
+      <c r="E251" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F251" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G251" t="n">
+        <v>0</v>
+      </c>
+      <c r="H251" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I251" t="n">
+        <v>0</v>
+      </c>
+      <c r="J251" t="n">
+        <v>21</v>
+      </c>
+      <c r="K251" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L251" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Lake Abert_01116755</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>608</v>
+      </c>
+      <c r="C252" t="n">
+        <v>54720000</v>
+      </c>
+      <c r="E252" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F252" t="n">
+        <v>654636.5</v>
+      </c>
+      <c r="G252" t="n">
+        <v>648326.92334</v>
+      </c>
+      <c r="H252" t="n">
+        <v>36060.7149586</v>
+      </c>
+      <c r="I252" t="n">
+        <v>72872.6033087</v>
+      </c>
+      <c r="J252" t="n">
+        <v>21</v>
+      </c>
+      <c r="K252" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L252" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Alkali Lake_01116863</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>29</v>
+      </c>
+      <c r="C253" t="n">
+        <v>2610000</v>
+      </c>
+      <c r="E253" t="n">
+        <v>222843.53125</v>
+      </c>
+      <c r="F253" t="n">
+        <v>1870683.625</v>
+      </c>
+      <c r="G253" t="n">
+        <v>1647840.09375</v>
+      </c>
+      <c r="H253" t="n">
+        <v>695088.037716</v>
+      </c>
+      <c r="I253" t="n">
+        <v>402851.102353</v>
+      </c>
+      <c r="J253" t="n">
+        <v>21</v>
+      </c>
+      <c r="K253" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L253" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Aspen Lake_01161255</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>36</v>
+      </c>
+      <c r="C254" t="n">
+        <v>3240000</v>
+      </c>
+      <c r="E254" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F254" t="n">
+        <v>173780.1875</v>
+      </c>
+      <c r="G254" t="n">
+        <v>167470.61084</v>
+      </c>
+      <c r="H254" t="n">
+        <v>47186.4604492</v>
+      </c>
+      <c r="I254" t="n">
+        <v>46339.734589</v>
+      </c>
+      <c r="J254" t="n">
+        <v>21</v>
+      </c>
+      <c r="K254" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L254" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Green Peter Lake_01158878</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>26</v>
+      </c>
+      <c r="C255" t="n">
+        <v>2340000</v>
+      </c>
+      <c r="E255" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F255" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G255" t="n">
+        <v>0</v>
+      </c>
+      <c r="H255" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I255" t="n">
+        <v>0</v>
+      </c>
+      <c r="J255" t="n">
+        <v>21</v>
+      </c>
+      <c r="K255" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L255" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Detroit Lake_01639301</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>31</v>
+      </c>
+      <c r="C256" t="n">
+        <v>2790000</v>
+      </c>
+      <c r="E256" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F256" t="n">
+        <v>23120.6640625</v>
+      </c>
+      <c r="G256" t="n">
+        <v>16811.0874023</v>
+      </c>
+      <c r="H256" t="n">
+        <v>7306.109312</v>
+      </c>
+      <c r="I256" t="n">
+        <v>3376.43008151</v>
+      </c>
+      <c r="J256" t="n">
+        <v>21</v>
+      </c>
+      <c r="K256" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L256" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Summer Lake_01150595</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>425</v>
+      </c>
+      <c r="C257" t="n">
+        <v>38250000</v>
+      </c>
+      <c r="E257" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F257" t="n">
+        <v>310456.03125</v>
+      </c>
+      <c r="G257" t="n">
+        <v>304146.45459</v>
+      </c>
+      <c r="H257" t="n">
+        <v>40555.7271967</v>
+      </c>
+      <c r="I257" t="n">
+        <v>51085.7504524</v>
+      </c>
+      <c r="J257" t="n">
+        <v>21</v>
+      </c>
+      <c r="K257" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L257" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Siltcoos Lake_01158483</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>98</v>
+      </c>
+      <c r="C258" t="n">
+        <v>8820000</v>
+      </c>
+      <c r="E258" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F258" t="n">
+        <v>285759.25</v>
+      </c>
+      <c r="G258" t="n">
+        <v>279449.67334</v>
+      </c>
+      <c r="H258" t="n">
+        <v>12748.8268595</v>
+      </c>
+      <c r="I258" t="n">
+        <v>31496.3731281</v>
+      </c>
+      <c r="J258" t="n">
+        <v>21</v>
+      </c>
+      <c r="K258" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L258" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Timothy Lake_01151253</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>4</v>
+      </c>
+      <c r="C259" t="n">
+        <v>360000</v>
+      </c>
+      <c r="E259" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F259" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G259" t="n">
+        <v>0</v>
+      </c>
+      <c r="H259" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I259" t="n">
+        <v>0</v>
+      </c>
+      <c r="J259" t="n">
+        <v>21</v>
+      </c>
+      <c r="K259" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L259" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Gerber Reservoir_01121105</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>9</v>
+      </c>
+      <c r="C260" t="n">
+        <v>810000</v>
+      </c>
+      <c r="E260" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F260" t="n">
+        <v>173780.1875</v>
+      </c>
+      <c r="G260" t="n">
+        <v>167470.61084</v>
+      </c>
+      <c r="H260" t="n">
+        <v>62713.5877821</v>
+      </c>
+      <c r="I260" t="n">
+        <v>50199.8539477</v>
+      </c>
+      <c r="J260" t="n">
+        <v>21</v>
+      </c>
+      <c r="K260" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L260" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Crater Lake_01163669</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>429</v>
+      </c>
+      <c r="C261" t="n">
+        <v>38610000</v>
+      </c>
+      <c r="E261" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F261" t="n">
+        <v>69823.296875</v>
+      </c>
+      <c r="G261" t="n">
+        <v>63513.7202148</v>
+      </c>
+      <c r="H261" t="n">
+        <v>7027.39298446</v>
+      </c>
+      <c r="I261" t="n">
+        <v>5190.30133663</v>
+      </c>
+      <c r="J261" t="n">
+        <v>21</v>
+      </c>
+      <c r="K261" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L261" s="12" t="n">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Lake Billy Chinook_01138120</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>109</v>
+      </c>
+      <c r="C262" t="n">
+        <v>9810000</v>
+      </c>
+      <c r="E262" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F262" t="n">
+        <v>89536.5078125</v>
+      </c>
+      <c r="G262" t="n">
+        <v>83226.93115230001</v>
+      </c>
+      <c r="H262" t="n">
+        <v>8800.428581030001</v>
+      </c>
+      <c r="I262" t="n">
+        <v>9737.051124170001</v>
+      </c>
+      <c r="J262" t="n">
+        <v>22</v>
+      </c>
+      <c r="K262" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L262" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Warm Springs Reservoir_01128656</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>75</v>
+      </c>
+      <c r="C263" t="n">
+        <v>6750000</v>
+      </c>
+      <c r="E263" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F263" t="n">
+        <v>114815.414062</v>
+      </c>
+      <c r="G263" t="n">
+        <v>108505.837402</v>
+      </c>
+      <c r="H263" t="n">
+        <v>10247.5363542</v>
+      </c>
+      <c r="I263" t="n">
+        <v>17017.8754608</v>
+      </c>
+      <c r="J263" t="n">
+        <v>22</v>
+      </c>
+      <c r="K263" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L263" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Beulah Reservoir_01117569</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>41</v>
+      </c>
+      <c r="C264" t="n">
+        <v>3690000</v>
+      </c>
+      <c r="E264" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F264" t="n">
+        <v>24434.3183594</v>
+      </c>
+      <c r="G264" t="n">
+        <v>18124.7416992</v>
+      </c>
+      <c r="H264" t="n">
+        <v>7066.90744093</v>
+      </c>
+      <c r="I264" t="n">
+        <v>3122.39563485</v>
+      </c>
+      <c r="J264" t="n">
+        <v>22</v>
+      </c>
+      <c r="K264" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L264" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Waldo Lake_01151818</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>237</v>
+      </c>
+      <c r="C265" t="n">
+        <v>21330000</v>
+      </c>
+      <c r="E265" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F265" t="n">
+        <v>328095.5</v>
+      </c>
+      <c r="G265" t="n">
+        <v>321785.92334</v>
+      </c>
+      <c r="H265" t="n">
+        <v>15931.4300748</v>
+      </c>
+      <c r="I265" t="n">
+        <v>27935.6186668</v>
+      </c>
+      <c r="J265" t="n">
+        <v>22</v>
+      </c>
+      <c r="K265" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L265" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Davis Lake_01140666</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>11</v>
+      </c>
+      <c r="C266" t="n">
+        <v>990000</v>
+      </c>
+      <c r="E266" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F266" t="n">
+        <v>159955.890625</v>
+      </c>
+      <c r="G266" t="n">
+        <v>153646.313965</v>
+      </c>
+      <c r="H266" t="n">
+        <v>53973.4037198</v>
+      </c>
+      <c r="I266" t="n">
+        <v>45459.4417852</v>
+      </c>
+      <c r="J266" t="n">
+        <v>22</v>
+      </c>
+      <c r="K266" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L266" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Crescent Lake_01158186</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>154</v>
+      </c>
+      <c r="C267" t="n">
+        <v>13860000</v>
+      </c>
+      <c r="E267" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F267" t="n">
+        <v>310456.03125</v>
+      </c>
+      <c r="G267" t="n">
+        <v>304146.45459</v>
+      </c>
+      <c r="H267" t="n">
+        <v>23761.7619978</v>
+      </c>
+      <c r="I267" t="n">
+        <v>58190.7777492</v>
+      </c>
+      <c r="J267" t="n">
+        <v>22</v>
+      </c>
+      <c r="K267" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L267" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Wickiup Reservoir_01161711</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>128</v>
+      </c>
+      <c r="C268" t="n">
+        <v>11520000</v>
+      </c>
+      <c r="E268" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F268" t="n">
+        <v>151356.234375</v>
+      </c>
+      <c r="G268" t="n">
+        <v>145046.657715</v>
+      </c>
+      <c r="H268" t="n">
+        <v>12458.6975708</v>
+      </c>
+      <c r="I268" t="n">
+        <v>18703.1638601</v>
+      </c>
+      <c r="J268" t="n">
+        <v>22</v>
+      </c>
+      <c r="K268" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L268" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Paulina Lake_01147502</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>57</v>
+      </c>
+      <c r="C269" t="n">
+        <v>5130000</v>
+      </c>
+      <c r="E269" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F269" t="n">
+        <v>43651.6171875</v>
+      </c>
+      <c r="G269" t="n">
+        <v>37342.0405273</v>
+      </c>
+      <c r="H269" t="n">
+        <v>7493.78805167</v>
+      </c>
+      <c r="I269" t="n">
+        <v>5980.62539666</v>
+      </c>
+      <c r="J269" t="n">
+        <v>22</v>
+      </c>
+      <c r="K269" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L269" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Odell Lake_01147159</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>138</v>
+      </c>
+      <c r="C270" t="n">
+        <v>12420000</v>
+      </c>
+      <c r="E270" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F270" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G270" t="n">
+        <v>0</v>
+      </c>
+      <c r="H270" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I270" t="n">
+        <v>0</v>
+      </c>
+      <c r="J270" t="n">
+        <v>22</v>
+      </c>
+      <c r="K270" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L270" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Crane Prairie Reservoir_01140386</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>8</v>
+      </c>
+      <c r="C271" t="n">
+        <v>720000</v>
+      </c>
+      <c r="E271" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F271" t="n">
+        <v>194088.640625</v>
+      </c>
+      <c r="G271" t="n">
+        <v>187779.063965</v>
+      </c>
+      <c r="H271" t="n">
+        <v>34088.3231812</v>
+      </c>
+      <c r="I271" t="n">
+        <v>61065.2046808</v>
+      </c>
+      <c r="J271" t="n">
+        <v>22</v>
+      </c>
+      <c r="K271" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L271" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Hills Creek Lake_01158881</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>62</v>
+      </c>
+      <c r="C272" t="n">
+        <v>5580000</v>
+      </c>
+      <c r="E272" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F272" t="n">
+        <v>277971.46875</v>
+      </c>
+      <c r="G272" t="n">
+        <v>271661.89209</v>
+      </c>
+      <c r="H272" t="n">
+        <v>13449.3357012</v>
+      </c>
+      <c r="I272" t="n">
+        <v>37910.2613977</v>
+      </c>
+      <c r="J272" t="n">
+        <v>22</v>
+      </c>
+      <c r="K272" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L272" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Lost Creek Lake_01158890</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>94</v>
+      </c>
+      <c r="C273" t="n">
+        <v>8460000</v>
+      </c>
+      <c r="E273" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F273" t="n">
+        <v>496592.40625</v>
+      </c>
+      <c r="G273" t="n">
+        <v>490282.82959</v>
+      </c>
+      <c r="H273" t="n">
+        <v>20140.9602259</v>
+      </c>
+      <c r="I273" t="n">
+        <v>65786.98994860001</v>
+      </c>
+      <c r="J273" t="n">
+        <v>22</v>
+      </c>
+      <c r="K273" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L273" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Malheur Lake_01123710</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>576</v>
+      </c>
+      <c r="C274" t="n">
+        <v>51840000</v>
+      </c>
+      <c r="E274" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F274" t="n">
+        <v>337287.5625</v>
+      </c>
+      <c r="G274" t="n">
+        <v>330977.98584</v>
+      </c>
+      <c r="H274" t="n">
+        <v>60896.0169152</v>
+      </c>
+      <c r="I274" t="n">
+        <v>67550.5392324</v>
+      </c>
+      <c r="J274" t="n">
+        <v>22</v>
+      </c>
+      <c r="K274" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L274" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Foster Lake_01158892</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>6</v>
+      </c>
+      <c r="C275" t="n">
+        <v>540000</v>
+      </c>
+      <c r="E275" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F275" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G275" t="n">
+        <v>0</v>
+      </c>
+      <c r="H275" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I275" t="n">
+        <v>0</v>
+      </c>
+      <c r="J275" t="n">
+        <v>22</v>
+      </c>
+      <c r="K275" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L275" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Goose Lake_00224325</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>402</v>
+      </c>
+      <c r="C276" t="n">
+        <v>36180000</v>
+      </c>
+      <c r="E276" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F276" t="n">
+        <v>173780.1875</v>
+      </c>
+      <c r="G276" t="n">
+        <v>167470.61084</v>
+      </c>
+      <c r="H276" t="n">
+        <v>25372.4847527</v>
+      </c>
+      <c r="I276" t="n">
+        <v>32296.4151639</v>
+      </c>
+      <c r="J276" t="n">
+        <v>22</v>
+      </c>
+      <c r="K276" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L276" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Upper Klamath Lake_01151685</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>2582</v>
+      </c>
+      <c r="C277" t="n">
+        <v>232380000</v>
+      </c>
+      <c r="E277" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F277" t="n">
+        <v>376704</v>
+      </c>
+      <c r="G277" t="n">
+        <v>370394.42334</v>
+      </c>
+      <c r="H277" t="n">
+        <v>11031.7559897</v>
+      </c>
+      <c r="I277" t="n">
+        <v>21869.0807816</v>
+      </c>
+      <c r="J277" t="n">
+        <v>22</v>
+      </c>
+      <c r="K277" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L277" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Lake Abert_01116755</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>730</v>
+      </c>
+      <c r="C278" t="n">
+        <v>65700000</v>
+      </c>
+      <c r="E278" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F278" t="n">
+        <v>619441.5</v>
+      </c>
+      <c r="G278" t="n">
+        <v>613131.92334</v>
+      </c>
+      <c r="H278" t="n">
+        <v>81364.5931333</v>
+      </c>
+      <c r="I278" t="n">
+        <v>71636.3643038</v>
+      </c>
+      <c r="J278" t="n">
+        <v>22</v>
+      </c>
+      <c r="K278" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L278" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Alkali Lake_01116863</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>29</v>
+      </c>
+      <c r="C279" t="n">
+        <v>2610000</v>
+      </c>
+      <c r="E279" t="n">
+        <v>14060.4824219</v>
+      </c>
+      <c r="F279" t="n">
+        <v>1541701.125</v>
+      </c>
+      <c r="G279" t="n">
+        <v>1527640.64258</v>
+      </c>
+      <c r="H279" t="n">
+        <v>580095.288591</v>
+      </c>
+      <c r="I279" t="n">
+        <v>402860.391445</v>
+      </c>
+      <c r="J279" t="n">
+        <v>22</v>
+      </c>
+      <c r="K279" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L279" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Aspen Lake_01161255</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>79</v>
+      </c>
+      <c r="C280" t="n">
+        <v>7110000</v>
+      </c>
+      <c r="E280" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F280" t="n">
+        <v>199526.3125</v>
+      </c>
+      <c r="G280" t="n">
+        <v>193216.73584</v>
+      </c>
+      <c r="H280" t="n">
+        <v>34524.6994042</v>
+      </c>
+      <c r="I280" t="n">
+        <v>47584.4917509</v>
+      </c>
+      <c r="J280" t="n">
+        <v>22</v>
+      </c>
+      <c r="K280" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L280" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Green Peter Lake_01158878</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>67</v>
+      </c>
+      <c r="C281" t="n">
+        <v>6030000</v>
+      </c>
+      <c r="E281" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F281" t="n">
+        <v>248885.8125</v>
+      </c>
+      <c r="G281" t="n">
+        <v>242576.23584</v>
+      </c>
+      <c r="H281" t="n">
+        <v>19562.5012608</v>
+      </c>
+      <c r="I281" t="n">
+        <v>41290.9277866</v>
+      </c>
+      <c r="J281" t="n">
+        <v>22</v>
+      </c>
+      <c r="K281" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L281" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Detroit Lake_01639301</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>65</v>
+      </c>
+      <c r="C282" t="n">
+        <v>5850000</v>
+      </c>
+      <c r="E282" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F282" t="n">
+        <v>139315.6875</v>
+      </c>
+      <c r="G282" t="n">
+        <v>133006.11084</v>
+      </c>
+      <c r="H282" t="n">
+        <v>17632.8858924</v>
+      </c>
+      <c r="I282" t="n">
+        <v>26807.4210891</v>
+      </c>
+      <c r="J282" t="n">
+        <v>22</v>
+      </c>
+      <c r="K282" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L282" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Summer Lake_01150595</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>1035</v>
+      </c>
+      <c r="C283" t="n">
+        <v>93150000</v>
+      </c>
+      <c r="E283" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F283" t="n">
+        <v>711213.875</v>
+      </c>
+      <c r="G283" t="n">
+        <v>704904.29834</v>
+      </c>
+      <c r="H283" t="n">
+        <v>74693.00773510001</v>
+      </c>
+      <c r="I283" t="n">
+        <v>109479.401916</v>
+      </c>
+      <c r="J283" t="n">
+        <v>22</v>
+      </c>
+      <c r="K283" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L283" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Siltcoos Lake_01158483</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>94</v>
+      </c>
+      <c r="C284" t="n">
+        <v>8460000</v>
+      </c>
+      <c r="E284" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F284" t="n">
+        <v>89536.5078125</v>
+      </c>
+      <c r="G284" t="n">
+        <v>83226.93115230001</v>
+      </c>
+      <c r="H284" t="n">
+        <v>9661.85817507</v>
+      </c>
+      <c r="I284" t="n">
+        <v>14043.050259</v>
+      </c>
+      <c r="J284" t="n">
+        <v>22</v>
+      </c>
+      <c r="K284" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L284" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Timothy Lake_01151253</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>20</v>
+      </c>
+      <c r="C285" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="E285" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F285" t="n">
+        <v>9549.926757810001</v>
+      </c>
+      <c r="G285" t="n">
+        <v>3240.35009766</v>
+      </c>
+      <c r="H285" t="n">
+        <v>6660.87692871</v>
+      </c>
+      <c r="I285" t="n">
+        <v>970.279796547</v>
+      </c>
+      <c r="J285" t="n">
+        <v>22</v>
+      </c>
+      <c r="K285" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L285" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Gerber Reservoir_01121105</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>7</v>
+      </c>
+      <c r="C286" t="n">
+        <v>630000</v>
+      </c>
+      <c r="E286" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F286" t="n">
+        <v>293765.0625</v>
+      </c>
+      <c r="G286" t="n">
+        <v>287455.48584</v>
+      </c>
+      <c r="H286" t="n">
+        <v>123026.070801</v>
+      </c>
+      <c r="I286" t="n">
+        <v>113613.44343</v>
+      </c>
+      <c r="J286" t="n">
+        <v>22</v>
+      </c>
+      <c r="K286" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L286" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Crater Lake_01163669</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>569</v>
+      </c>
+      <c r="C287" t="n">
+        <v>51210000</v>
+      </c>
+      <c r="E287" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F287" t="n">
+        <v>301995.375</v>
+      </c>
+      <c r="G287" t="n">
+        <v>295685.79834</v>
+      </c>
+      <c r="H287" t="n">
+        <v>10855.3888444</v>
+      </c>
+      <c r="I287" t="n">
+        <v>22141.7484073</v>
+      </c>
+      <c r="J287" t="n">
+        <v>22</v>
+      </c>
+      <c r="K287" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L287" s="12" t="n">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Lake Billy Chinook_01138120</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>91</v>
+      </c>
+      <c r="C288" t="n">
+        <v>8190000</v>
+      </c>
+      <c r="E288" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F288" t="n">
+        <v>255858.734375</v>
+      </c>
+      <c r="G288" t="n">
+        <v>249549.157715</v>
+      </c>
+      <c r="H288" t="n">
+        <v>21090.1777075</v>
+      </c>
+      <c r="I288" t="n">
+        <v>39988.4714188</v>
+      </c>
+      <c r="J288" t="n">
+        <v>23</v>
+      </c>
+      <c r="K288" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L288" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Waldo Lake_01151818</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>211</v>
+      </c>
+      <c r="C289" t="n">
+        <v>18990000</v>
+      </c>
+      <c r="E289" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F289" t="n">
+        <v>346737</v>
+      </c>
+      <c r="G289" t="n">
+        <v>340427.42334</v>
+      </c>
+      <c r="H289" t="n">
+        <v>32496.0096268</v>
+      </c>
+      <c r="I289" t="n">
+        <v>46197.0726724</v>
+      </c>
+      <c r="J289" t="n">
+        <v>23</v>
+      </c>
+      <c r="K289" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L289" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Davis Lake_01140666</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>16</v>
+      </c>
+      <c r="C290" t="n">
+        <v>1440000</v>
+      </c>
+      <c r="E290" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F290" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G290" t="n">
+        <v>0</v>
+      </c>
+      <c r="H290" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I290" t="n">
+        <v>0</v>
+      </c>
+      <c r="J290" t="n">
+        <v>23</v>
+      </c>
+      <c r="K290" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L290" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Crescent Lake_01158186</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>112</v>
+      </c>
+      <c r="C291" t="n">
+        <v>10080000</v>
+      </c>
+      <c r="E291" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F291" t="n">
+        <v>319153.9375</v>
+      </c>
+      <c r="G291" t="n">
+        <v>312844.36084</v>
+      </c>
+      <c r="H291" t="n">
+        <v>25982.1876046</v>
+      </c>
+      <c r="I291" t="n">
+        <v>54079.2379703</v>
+      </c>
+      <c r="J291" t="n">
+        <v>23</v>
+      </c>
+      <c r="K291" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L291" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Wickiup Reservoir_01161711</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>116</v>
+      </c>
+      <c r="C292" t="n">
+        <v>10440000</v>
+      </c>
+      <c r="E292" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F292" t="n">
+        <v>114815.414062</v>
+      </c>
+      <c r="G292" t="n">
+        <v>108505.837402</v>
+      </c>
+      <c r="H292" t="n">
+        <v>15989.8944302</v>
+      </c>
+      <c r="I292" t="n">
+        <v>22730.3720487</v>
+      </c>
+      <c r="J292" t="n">
+        <v>23</v>
+      </c>
+      <c r="K292" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L292" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Paulina Lake_01147502</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>53</v>
+      </c>
+      <c r="C293" t="n">
+        <v>4770000</v>
+      </c>
+      <c r="E293" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F293" t="n">
+        <v>483059.09375</v>
+      </c>
+      <c r="G293" t="n">
+        <v>476749.51709</v>
+      </c>
+      <c r="H293" t="n">
+        <v>33095.1257094</v>
+      </c>
+      <c r="I293" t="n">
+        <v>100857.643583</v>
+      </c>
+      <c r="J293" t="n">
+        <v>23</v>
+      </c>
+      <c r="K293" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L293" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Odell Lake_01147159</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>135</v>
+      </c>
+      <c r="C294" t="n">
+        <v>12150000</v>
+      </c>
+      <c r="E294" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F294" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G294" t="n">
+        <v>0</v>
+      </c>
+      <c r="H294" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I294" t="n">
+        <v>0</v>
+      </c>
+      <c r="J294" t="n">
+        <v>23</v>
+      </c>
+      <c r="K294" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L294" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Cottage Grove Lake_01158179</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>8</v>
+      </c>
+      <c r="C295" t="n">
+        <v>720000</v>
+      </c>
+      <c r="E295" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F295" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G295" t="n">
+        <v>0</v>
+      </c>
+      <c r="H295" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I295" t="n">
+        <v>0</v>
+      </c>
+      <c r="J295" t="n">
+        <v>23</v>
+      </c>
+      <c r="K295" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L295" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Dorena Lake_01120032</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>19</v>
+      </c>
+      <c r="C296" t="n">
+        <v>1710000</v>
+      </c>
+      <c r="E296" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F296" t="n">
+        <v>51522.8789062</v>
+      </c>
+      <c r="G296" t="n">
+        <v>45213.3022461</v>
+      </c>
+      <c r="H296" t="n">
+        <v>11196.9028577</v>
+      </c>
+      <c r="I296" t="n">
+        <v>11995.8607127</v>
+      </c>
+      <c r="J296" t="n">
+        <v>23</v>
+      </c>
+      <c r="K296" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L296" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Hills Creek Lake_01158881</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>51</v>
+      </c>
+      <c r="C297" t="n">
+        <v>4590000</v>
+      </c>
+      <c r="E297" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F297" t="n">
+        <v>159955.890625</v>
+      </c>
+      <c r="G297" t="n">
+        <v>153646.313965</v>
+      </c>
+      <c r="H297" t="n">
+        <v>12425.9895067</v>
+      </c>
+      <c r="I297" t="n">
+        <v>27485.3764501</v>
+      </c>
+      <c r="J297" t="n">
+        <v>23</v>
+      </c>
+      <c r="K297" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L297" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Lost Creek Lake_01158890</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>92</v>
+      </c>
+      <c r="C298" t="n">
+        <v>8280000</v>
+      </c>
+      <c r="E298" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F298" t="n">
+        <v>346737</v>
+      </c>
+      <c r="G298" t="n">
+        <v>340427.42334</v>
+      </c>
+      <c r="H298" t="n">
+        <v>11871.8062797</v>
+      </c>
+      <c r="I298" t="n">
+        <v>36478.7102919</v>
+      </c>
+      <c r="J298" t="n">
+        <v>23</v>
+      </c>
+      <c r="K298" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L298" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Malheur Lake_01123710</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>579</v>
+      </c>
+      <c r="C299" t="n">
+        <v>52110000</v>
+      </c>
+      <c r="E299" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F299" t="n">
+        <v>310456.03125</v>
+      </c>
+      <c r="G299" t="n">
+        <v>304146.45459</v>
+      </c>
+      <c r="H299" t="n">
+        <v>45773.6557836</v>
+      </c>
+      <c r="I299" t="n">
+        <v>55201.5696545</v>
+      </c>
+      <c r="J299" t="n">
+        <v>23</v>
+      </c>
+      <c r="K299" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L299" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Foster Lake_01158892</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>28</v>
+      </c>
+      <c r="C300" t="n">
+        <v>2520000</v>
+      </c>
+      <c r="E300" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F300" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G300" t="n">
+        <v>0</v>
+      </c>
+      <c r="H300" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I300" t="n">
+        <v>0</v>
+      </c>
+      <c r="J300" t="n">
+        <v>23</v>
+      </c>
+      <c r="K300" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L300" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Goose Lake_00224325</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>333</v>
+      </c>
+      <c r="C301" t="n">
+        <v>29970000</v>
+      </c>
+      <c r="E301" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F301" t="n">
+        <v>178648.890625</v>
+      </c>
+      <c r="G301" t="n">
+        <v>172339.313965</v>
+      </c>
+      <c r="H301" t="n">
+        <v>18567.6215058</v>
+      </c>
+      <c r="I301" t="n">
+        <v>26433.4307449</v>
+      </c>
+      <c r="J301" t="n">
+        <v>23</v>
+      </c>
+      <c r="K301" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L301" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Upper Klamath Lake_01151685</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>2559</v>
+      </c>
+      <c r="C302" t="n">
+        <v>230310000</v>
+      </c>
+      <c r="E302" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F302" t="n">
+        <v>496592.40625</v>
+      </c>
+      <c r="G302" t="n">
+        <v>490282.82959</v>
+      </c>
+      <c r="H302" t="n">
+        <v>10805.4020026</v>
+      </c>
+      <c r="I302" t="n">
+        <v>26297.310113</v>
+      </c>
+      <c r="J302" t="n">
+        <v>23</v>
+      </c>
+      <c r="K302" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L302" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Henry Hagg Lake_01158095</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>27</v>
+      </c>
+      <c r="C303" t="n">
+        <v>2430000</v>
+      </c>
+      <c r="E303" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F303" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G303" t="n">
+        <v>0</v>
+      </c>
+      <c r="H303" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I303" t="n">
+        <v>0</v>
+      </c>
+      <c r="J303" t="n">
+        <v>23</v>
+      </c>
+      <c r="K303" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L303" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Lake Abert_01116755</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>796</v>
+      </c>
+      <c r="C304" t="n">
+        <v>71640000</v>
+      </c>
+      <c r="E304" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F304" t="n">
+        <v>636795.75</v>
+      </c>
+      <c r="G304" t="n">
+        <v>630486.17334</v>
+      </c>
+      <c r="H304" t="n">
+        <v>74079.3892681</v>
+      </c>
+      <c r="I304" t="n">
+        <v>71471.93327179999</v>
+      </c>
+      <c r="J304" t="n">
+        <v>23</v>
+      </c>
+      <c r="K304" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L304" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Alkali Lake_01116863</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>29</v>
+      </c>
+      <c r="C305" t="n">
+        <v>2610000</v>
+      </c>
+      <c r="E305" t="n">
+        <v>20137.2480469</v>
+      </c>
+      <c r="F305" t="n">
+        <v>1819701.875</v>
+      </c>
+      <c r="G305" t="n">
+        <v>1799564.62695</v>
+      </c>
+      <c r="H305" t="n">
+        <v>689824.194976</v>
+      </c>
+      <c r="I305" t="n">
+        <v>457760.505526</v>
+      </c>
+      <c r="J305" t="n">
+        <v>23</v>
+      </c>
+      <c r="K305" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L305" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Aspen Lake_01161255</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>50</v>
+      </c>
+      <c r="C306" t="n">
+        <v>4500000</v>
+      </c>
+      <c r="E306" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F306" t="n">
+        <v>169044.15625</v>
+      </c>
+      <c r="G306" t="n">
+        <v>162734.57959</v>
+      </c>
+      <c r="H306" t="n">
+        <v>23829.7345215</v>
+      </c>
+      <c r="I306" t="n">
+        <v>43807.1625964</v>
+      </c>
+      <c r="J306" t="n">
+        <v>23</v>
+      </c>
+      <c r="K306" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L306" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Green Peter Lake_01158878</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>74</v>
+      </c>
+      <c r="C307" t="n">
+        <v>6660000</v>
+      </c>
+      <c r="E307" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F307" t="n">
+        <v>816582.6875</v>
+      </c>
+      <c r="G307" t="n">
+        <v>810273.11084</v>
+      </c>
+      <c r="H307" t="n">
+        <v>65368.2108055</v>
+      </c>
+      <c r="I307" t="n">
+        <v>156159.612028</v>
+      </c>
+      <c r="J307" t="n">
+        <v>23</v>
+      </c>
+      <c r="K307" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L307" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Detroit Lake_01639301</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>58</v>
+      </c>
+      <c r="C308" t="n">
+        <v>5220000</v>
+      </c>
+      <c r="E308" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F308" t="n">
+        <v>164437.203125</v>
+      </c>
+      <c r="G308" t="n">
+        <v>158127.626465</v>
+      </c>
+      <c r="H308" t="n">
+        <v>23956.9033624</v>
+      </c>
+      <c r="I308" t="n">
+        <v>35629.0257942</v>
+      </c>
+      <c r="J308" t="n">
+        <v>23</v>
+      </c>
+      <c r="K308" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L308" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Summer Lake_01150595</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>1046</v>
+      </c>
+      <c r="C309" t="n">
+        <v>94140000</v>
+      </c>
+      <c r="E309" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F309" t="n">
+        <v>772681.0625</v>
+      </c>
+      <c r="G309" t="n">
+        <v>766371.48584</v>
+      </c>
+      <c r="H309" t="n">
+        <v>69937.47913180001</v>
+      </c>
+      <c r="I309" t="n">
+        <v>104394.525833</v>
+      </c>
+      <c r="J309" t="n">
+        <v>23</v>
+      </c>
+      <c r="K309" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L309" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Siltcoos Lake_01158483</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>117</v>
+      </c>
+      <c r="C310" t="n">
+        <v>10530000</v>
+      </c>
+      <c r="E310" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F310" t="n">
+        <v>1270574.375</v>
+      </c>
+      <c r="G310" t="n">
+        <v>1264264.79834</v>
+      </c>
+      <c r="H310" t="n">
+        <v>38709.1678602</v>
+      </c>
+      <c r="I310" t="n">
+        <v>140494.135767</v>
+      </c>
+      <c r="J310" t="n">
+        <v>23</v>
+      </c>
+      <c r="K310" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L310" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Timothy Lake_01151253</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>18</v>
+      </c>
+      <c r="C311" t="n">
+        <v>1620000</v>
+      </c>
+      <c r="E311" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F311" t="n">
+        <v>912011.4375</v>
+      </c>
+      <c r="G311" t="n">
+        <v>905701.86084</v>
+      </c>
+      <c r="H311" t="n">
+        <v>115809.217095</v>
+      </c>
+      <c r="I311" t="n">
+        <v>239067.331083</v>
+      </c>
+      <c r="J311" t="n">
+        <v>23</v>
+      </c>
+      <c r="K311" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L311" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Gerber Reservoir_01121105</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>12</v>
+      </c>
+      <c r="C312" t="n">
+        <v>1080000</v>
+      </c>
+      <c r="E312" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F312" t="n">
+        <v>301995.375</v>
+      </c>
+      <c r="G312" t="n">
+        <v>295685.79834</v>
+      </c>
+      <c r="H312" t="n">
+        <v>100282.358073</v>
+      </c>
+      <c r="I312" t="n">
+        <v>104044.68877</v>
+      </c>
+      <c r="J312" t="n">
+        <v>23</v>
+      </c>
+      <c r="K312" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L312" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Crater Lake_01163669</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>479</v>
+      </c>
+      <c r="C313" t="n">
+        <v>43110000</v>
+      </c>
+      <c r="E313" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F313" t="n">
+        <v>420726.6875</v>
+      </c>
+      <c r="G313" t="n">
+        <v>414417.11084</v>
+      </c>
+      <c r="H313" t="n">
+        <v>17438.0115332</v>
+      </c>
+      <c r="I313" t="n">
+        <v>29652.774446</v>
+      </c>
+      <c r="J313" t="n">
+        <v>23</v>
+      </c>
+      <c r="K313" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L313" s="12" t="n">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Lake Billy Chinook_01138120</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>82</v>
+      </c>
+      <c r="C314" t="n">
+        <v>7380000</v>
+      </c>
+      <c r="D314" t="inlineStr"/>
+      <c r="E314" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F314" t="n">
+        <v>67920.3984375</v>
+      </c>
+      <c r="G314" t="n">
+        <v>61610.8217773</v>
+      </c>
+      <c r="H314" t="n">
+        <v>8084.72612186</v>
+      </c>
+      <c r="I314" t="n">
+        <v>8961.43257243</v>
+      </c>
+      <c r="J314" t="n">
+        <v>24</v>
+      </c>
+      <c r="K314" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L314" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Waldo Lake_01151818</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>239</v>
+      </c>
+      <c r="C315" t="n">
+        <v>21510000</v>
+      </c>
+      <c r="D315" t="inlineStr"/>
+      <c r="E315" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F315" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G315" t="n">
+        <v>0</v>
+      </c>
+      <c r="H315" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I315" t="n">
+        <v>0</v>
+      </c>
+      <c r="J315" t="n">
+        <v>24</v>
+      </c>
+      <c r="K315" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L315" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Davis Lake_01140666</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>13</v>
+      </c>
+      <c r="C316" t="n">
+        <v>1170000</v>
+      </c>
+      <c r="D316" t="inlineStr"/>
+      <c r="E316" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F316" t="n">
+        <v>94623.78125</v>
+      </c>
+      <c r="G316" t="n">
+        <v>88314.20458980001</v>
+      </c>
+      <c r="H316" t="n">
+        <v>13102.9770132</v>
+      </c>
+      <c r="I316" t="n">
+        <v>23533.0291353</v>
+      </c>
+      <c r="J316" t="n">
+        <v>24</v>
+      </c>
+      <c r="K316" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L316" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Fern Ridge Lake_01120678</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>17</v>
+      </c>
+      <c r="C317" t="n">
+        <v>1530000</v>
+      </c>
+      <c r="D317" t="inlineStr"/>
+      <c r="E317" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F317" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G317" t="n">
+        <v>0</v>
+      </c>
+      <c r="H317" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I317" t="n">
+        <v>0</v>
+      </c>
+      <c r="J317" t="n">
+        <v>24</v>
+      </c>
+      <c r="K317" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L317" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Crescent Lake_01158186</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>145</v>
+      </c>
+      <c r="C318" t="n">
+        <v>13050000</v>
+      </c>
+      <c r="D318" t="inlineStr"/>
+      <c r="E318" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F318" t="n">
+        <v>23768.4121094</v>
+      </c>
+      <c r="G318" t="n">
+        <v>17458.8354492</v>
+      </c>
+      <c r="H318" t="n">
+        <v>6551.08871228</v>
+      </c>
+      <c r="I318" t="n">
+        <v>1773.29346248</v>
+      </c>
+      <c r="J318" t="n">
+        <v>24</v>
+      </c>
+      <c r="K318" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L318" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Wickiup Reservoir_01161711</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>124</v>
+      </c>
+      <c r="C319" t="n">
+        <v>11160000</v>
+      </c>
+      <c r="D319" t="inlineStr"/>
+      <c r="E319" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F319" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G319" t="n">
+        <v>0</v>
+      </c>
+      <c r="H319" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I319" t="n">
+        <v>0</v>
+      </c>
+      <c r="J319" t="n">
+        <v>24</v>
+      </c>
+      <c r="K319" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L319" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Paulina Lake_01147502</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>57</v>
+      </c>
+      <c r="C320" t="n">
+        <v>5130000</v>
+      </c>
+      <c r="D320" t="inlineStr"/>
+      <c r="E320" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F320" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G320" t="n">
+        <v>0</v>
+      </c>
+      <c r="H320" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I320" t="n">
+        <v>0</v>
+      </c>
+      <c r="J320" t="n">
+        <v>24</v>
+      </c>
+      <c r="K320" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L320" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Odell Lake_01147159</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>136</v>
+      </c>
+      <c r="C321" t="n">
+        <v>12240000</v>
+      </c>
+      <c r="D321" t="inlineStr"/>
+      <c r="E321" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F321" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G321" t="n">
+        <v>0</v>
+      </c>
+      <c r="H321" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I321" t="n">
+        <v>0</v>
+      </c>
+      <c r="J321" t="n">
+        <v>24</v>
+      </c>
+      <c r="K321" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L321" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Cottage Grove Lake_01158179</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>12</v>
+      </c>
+      <c r="C322" t="n">
+        <v>1080000</v>
+      </c>
+      <c r="D322" t="inlineStr"/>
+      <c r="E322" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F322" t="n">
+        <v>75857.78125</v>
+      </c>
+      <c r="G322" t="n">
+        <v>69548.20458980001</v>
+      </c>
+      <c r="H322" t="n">
+        <v>15423.7777507</v>
+      </c>
+      <c r="I322" t="n">
+        <v>21264.0877086</v>
+      </c>
+      <c r="J322" t="n">
+        <v>24</v>
+      </c>
+      <c r="K322" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L322" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Dorena Lake_01120032</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>19</v>
+      </c>
+      <c r="C323" t="n">
+        <v>1710000</v>
+      </c>
+      <c r="D323" t="inlineStr"/>
+      <c r="E323" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F323" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G323" t="n">
+        <v>0</v>
+      </c>
+      <c r="H323" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I323" t="n">
+        <v>0</v>
+      </c>
+      <c r="J323" t="n">
+        <v>24</v>
+      </c>
+      <c r="K323" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L323" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Hills Creek Lake_01158881</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>58</v>
+      </c>
+      <c r="C324" t="n">
+        <v>5220000</v>
+      </c>
+      <c r="D324" t="inlineStr"/>
+      <c r="E324" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F324" t="n">
+        <v>135519</v>
+      </c>
+      <c r="G324" t="n">
+        <v>129209.42334</v>
+      </c>
+      <c r="H324" t="n">
+        <v>9858.33929654</v>
+      </c>
+      <c r="I324" t="n">
+        <v>17697.8240326</v>
+      </c>
+      <c r="J324" t="n">
+        <v>24</v>
+      </c>
+      <c r="K324" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L324" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Lost Creek Lake_01158890</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>51</v>
+      </c>
+      <c r="C325" t="n">
+        <v>4590000</v>
+      </c>
+      <c r="D325" t="inlineStr"/>
+      <c r="E325" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F325" t="n">
+        <v>337287.5625</v>
+      </c>
+      <c r="G325" t="n">
+        <v>330977.98584</v>
+      </c>
+      <c r="H325" t="n">
+        <v>32862.4444891</v>
+      </c>
+      <c r="I325" t="n">
+        <v>69096.2393508</v>
+      </c>
+      <c r="J325" t="n">
+        <v>24</v>
+      </c>
+      <c r="K325" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L325" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Malheur Lake_01123710</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>569</v>
+      </c>
+      <c r="C326" t="n">
+        <v>51210000</v>
+      </c>
+      <c r="D326" t="inlineStr"/>
+      <c r="E326" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F326" t="n">
+        <v>366437.6875</v>
+      </c>
+      <c r="G326" t="n">
+        <v>360128.11084</v>
+      </c>
+      <c r="H326" t="n">
+        <v>66193.9407086</v>
+      </c>
+      <c r="I326" t="n">
+        <v>76139.0798914</v>
+      </c>
+      <c r="J326" t="n">
+        <v>24</v>
+      </c>
+      <c r="K326" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L326" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Foster Lake_01158892</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>29</v>
+      </c>
+      <c r="C327" t="n">
+        <v>2610000</v>
+      </c>
+      <c r="D327" t="inlineStr"/>
+      <c r="E327" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F327" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G327" t="n">
+        <v>0</v>
+      </c>
+      <c r="H327" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I327" t="n">
+        <v>0</v>
+      </c>
+      <c r="J327" t="n">
+        <v>24</v>
+      </c>
+      <c r="K327" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L327" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Goose Lake_00224325</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>224</v>
+      </c>
+      <c r="C328" t="n">
+        <v>20160000</v>
+      </c>
+      <c r="D328" t="inlineStr"/>
+      <c r="E328" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F328" t="n">
+        <v>277971.46875</v>
+      </c>
+      <c r="G328" t="n">
+        <v>271661.89209</v>
+      </c>
+      <c r="H328" t="n">
+        <v>41274.3708496</v>
+      </c>
+      <c r="I328" t="n">
+        <v>56265.0297647</v>
+      </c>
+      <c r="J328" t="n">
+        <v>24</v>
+      </c>
+      <c r="K328" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L328" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Upper Klamath Lake_01151685</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>2469</v>
+      </c>
+      <c r="C329" t="n">
+        <v>222210000</v>
+      </c>
+      <c r="D329" t="inlineStr"/>
+      <c r="E329" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F329" t="n">
+        <v>398107.53125</v>
+      </c>
+      <c r="G329" t="n">
+        <v>391797.95459</v>
+      </c>
+      <c r="H329" t="n">
+        <v>9469.95847731</v>
+      </c>
+      <c r="I329" t="n">
+        <v>18672.7235144</v>
+      </c>
+      <c r="J329" t="n">
+        <v>24</v>
+      </c>
+      <c r="K329" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L329" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Lake Abert_01116755</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>589</v>
+      </c>
+      <c r="C330" t="n">
+        <v>53010000</v>
+      </c>
+      <c r="D330" t="inlineStr"/>
+      <c r="E330" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F330" t="n">
+        <v>376704</v>
+      </c>
+      <c r="G330" t="n">
+        <v>370394.42334</v>
+      </c>
+      <c r="H330" t="n">
+        <v>92595.1851821</v>
+      </c>
+      <c r="I330" t="n">
+        <v>68647.3970441</v>
+      </c>
+      <c r="J330" t="n">
+        <v>24</v>
+      </c>
+      <c r="K330" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L330" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Alkali Lake_01116863</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>29</v>
+      </c>
+      <c r="C331" t="n">
+        <v>2610000</v>
+      </c>
+      <c r="D331" t="inlineStr"/>
+      <c r="E331" t="n">
+        <v>34040.8242188</v>
+      </c>
+      <c r="F331" t="n">
+        <v>1306171.375</v>
+      </c>
+      <c r="G331" t="n">
+        <v>1272130.55078</v>
+      </c>
+      <c r="H331" t="n">
+        <v>340644.599811</v>
+      </c>
+      <c r="I331" t="n">
+        <v>321379.895319</v>
+      </c>
+      <c r="J331" t="n">
+        <v>24</v>
+      </c>
+      <c r="K331" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L331" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Aspen Lake_01161255</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>70</v>
+      </c>
+      <c r="C332" t="n">
+        <v>6300000</v>
+      </c>
+      <c r="D332" t="inlineStr"/>
+      <c r="E332" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F332" t="n">
+        <v>229086.84375</v>
+      </c>
+      <c r="G332" t="n">
+        <v>222777.26709</v>
+      </c>
+      <c r="H332" t="n">
+        <v>28332.2958078</v>
+      </c>
+      <c r="I332" t="n">
+        <v>44377.8881601</v>
+      </c>
+      <c r="J332" t="n">
+        <v>24</v>
+      </c>
+      <c r="K332" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L332" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Green Peter Lake_01158878</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>89</v>
+      </c>
+      <c r="C333" t="n">
+        <v>8010000</v>
+      </c>
+      <c r="D333" t="inlineStr"/>
+      <c r="E333" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F333" t="n">
+        <v>420726.6875</v>
+      </c>
+      <c r="G333" t="n">
+        <v>414417.11084</v>
+      </c>
+      <c r="H333" t="n">
+        <v>24938.3895003</v>
+      </c>
+      <c r="I333" t="n">
+        <v>56881.9736832</v>
+      </c>
+      <c r="J333" t="n">
+        <v>24</v>
+      </c>
+      <c r="K333" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L333" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Detroit Lake_01639301</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>52</v>
+      </c>
+      <c r="C334" t="n">
+        <v>4680000</v>
+      </c>
+      <c r="D334" t="inlineStr"/>
+      <c r="E334" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F334" t="n">
+        <v>60813.5234375</v>
+      </c>
+      <c r="G334" t="n">
+        <v>54503.9467773</v>
+      </c>
+      <c r="H334" t="n">
+        <v>9053.5499831</v>
+      </c>
+      <c r="I334" t="n">
+        <v>9959.5752017</v>
+      </c>
+      <c r="J334" t="n">
+        <v>24</v>
+      </c>
+      <c r="K334" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L334" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Summer Lake_01150595</t>
+        </is>
+      </c>
+      <c r="B335" t="n">
+        <v>1122</v>
+      </c>
+      <c r="C335" t="n">
+        <v>100980000</v>
+      </c>
+      <c r="D335" t="inlineStr"/>
+      <c r="E335" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F335" t="n">
+        <v>554626</v>
+      </c>
+      <c r="G335" t="n">
+        <v>548316.42334</v>
+      </c>
+      <c r="H335" t="n">
+        <v>46943.9501213</v>
+      </c>
+      <c r="I335" t="n">
+        <v>80084.2476819</v>
+      </c>
+      <c r="J335" t="n">
+        <v>24</v>
+      </c>
+      <c r="K335" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L335" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>Siltcoos Lake_01158483</t>
+        </is>
+      </c>
+      <c r="B336" t="n">
+        <v>104</v>
+      </c>
+      <c r="C336" t="n">
+        <v>9360000</v>
+      </c>
+      <c r="D336" t="inlineStr"/>
+      <c r="E336" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F336" t="n">
+        <v>356451.15625</v>
+      </c>
+      <c r="G336" t="n">
+        <v>350141.57959</v>
+      </c>
+      <c r="H336" t="n">
+        <v>24900.551894</v>
+      </c>
+      <c r="I336" t="n">
+        <v>61599.2967602</v>
+      </c>
+      <c r="J336" t="n">
+        <v>24</v>
+      </c>
+      <c r="K336" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L336" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Howard Prairie Lake_01158895</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>5</v>
+      </c>
+      <c r="C337" t="n">
+        <v>450000</v>
+      </c>
+      <c r="D337" t="inlineStr"/>
+      <c r="E337" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F337" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G337" t="n">
+        <v>0</v>
+      </c>
+      <c r="H337" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I337" t="n">
+        <v>0</v>
+      </c>
+      <c r="J337" t="n">
+        <v>24</v>
+      </c>
+      <c r="K337" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L337" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>Timothy Lake_01151253</t>
+        </is>
+      </c>
+      <c r="B338" t="n">
+        <v>14</v>
+      </c>
+      <c r="C338" t="n">
+        <v>1260000</v>
+      </c>
+      <c r="D338" t="inlineStr"/>
+      <c r="E338" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F338" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="G338" t="n">
+        <v>0</v>
+      </c>
+      <c r="H338" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="I338" t="n">
+        <v>0</v>
+      </c>
+      <c r="J338" t="n">
+        <v>24</v>
+      </c>
+      <c r="K338" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L338" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Gerber Reservoir_01121105</t>
+        </is>
+      </c>
+      <c r="B339" t="n">
+        <v>14</v>
+      </c>
+      <c r="C339" t="n">
+        <v>1260000</v>
+      </c>
+      <c r="D339" t="inlineStr"/>
+      <c r="E339" t="n">
+        <v>12589.2578125</v>
+      </c>
+      <c r="F339" t="n">
+        <v>229086.84375</v>
+      </c>
+      <c r="G339" t="n">
+        <v>216497.585938</v>
+      </c>
+      <c r="H339" t="n">
+        <v>58357.6095843</v>
+      </c>
+      <c r="I339" t="n">
+        <v>55279.6924044</v>
+      </c>
+      <c r="J339" t="n">
+        <v>24</v>
+      </c>
+      <c r="K339" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L339" s="12" t="n">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Crater Lake_01163669</t>
+        </is>
+      </c>
+      <c r="B340" t="n">
+        <v>569</v>
+      </c>
+      <c r="C340" t="n">
+        <v>51210000</v>
+      </c>
+      <c r="D340" t="inlineStr"/>
+      <c r="E340" t="n">
+        <v>6309.57666016</v>
+      </c>
+      <c r="F340" t="n">
+        <v>24434.3183594</v>
+      </c>
+      <c r="G340" t="n">
+        <v>18124.7416992</v>
+      </c>
+      <c r="H340" t="n">
+        <v>6357.05186937</v>
+      </c>
+      <c r="I340" t="n">
+        <v>826.403904853</v>
+      </c>
+      <c r="J340" t="n">
+        <v>24</v>
+      </c>
+      <c r="K340" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L340" s="12" t="n">
+        <v>44585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>